<commit_message>
Deploying to gh-pages from @ GA4GH-Pedigree-Standard/pedigree-fhir-ig@ac8e0a6cc8d299bc1d587051b846e25c8905508f 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-Pedigree.xlsx
+++ b/StructureDefinition-Pedigree.xlsx
@@ -1176,7 +1176,7 @@
     <t>Composition.section</t>
   </si>
   <si>
-    <t>5</t>
+    <t>4</t>
   </si>
   <si>
     <t>Composition is broken into sections</t>
@@ -15671,7 +15671,7 @@
       </c>
       <c r="D123" s="2"/>
       <c r="E123" t="s" s="2">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F123" t="s" s="2">
         <v>53</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ GA4GH-Pedigree-Standard/pedigree-fhir-ig@21ccf8c044ce825569eb3b882ca81723e169f9b8 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-Pedigree.xlsx
+++ b/StructureDefinition-Pedigree.xlsx
@@ -1412,13 +1412,13 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
+    &lt;system value="http://purl.org/ga4gh/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
     &lt;code value="proband"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ga4gh-cp.github.io/pedigree-fhir-ig/StructureDefinition/PedigreeIndividual)
+    <t xml:space="preserve">Reference(http://purl.org/ga4gh/pedigree-fhir-ig/StructureDefinition/PedigreeIndividual)
 </t>
   </si>
   <si>
@@ -1430,7 +1430,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
+    &lt;system value="http://purl.org/ga4gh/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
     &lt;code value="reason"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
@@ -1448,7 +1448,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
+    &lt;system value="http://purl.org/ga4gh/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
     &lt;code value="individuals"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
@@ -1462,13 +1462,13 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
+    &lt;system value="http://purl.org/ga4gh/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
     &lt;code value="relationships"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ga4gh-cp.github.io/pedigree-fhir-ig/StructureDefinition/PedigreeRelationship)
+    <t xml:space="preserve">Reference(http://purl.org/ga4gh/pedigree-fhir-ig/StructureDefinition/PedigreeRelationship)
 </t>
   </si>
   <si>
@@ -1480,7 +1480,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
+    &lt;system value="http://purl.org/ga4gh/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
     &lt;code value="other"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>

</xml_diff>